<commit_message>
updated Misc and metadata
</commit_message>
<xml_diff>
--- a/PDFs_experimental/MetaData.xlsx
+++ b/PDFs_experimental/MetaData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andysodeanker/Documents/Materiale_Kemi_new/Materiale_Kemi/Co-Author/ICLR/PDFs_experimental/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andysodeanker/Downloads/InOrgMatDataset/PDFs_experimental/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{22A8D4A8-D1D1-7F47-90DC-34D50945BD2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{958A1A66-36CB-3D4A-A782-59BAA1A0CC7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-12660" yWindow="-28300" windowWidth="51200" windowHeight="28300" xr2:uid="{26E4C037-BF76-1448-992E-3DD870856628}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="54">
   <si>
     <t>Datafile</t>
   </si>
@@ -169,6 +169,33 @@
   </si>
   <si>
     <t>10.1021/acsomega.8b01613</t>
+  </si>
+  <si>
+    <t>0.7</t>
+  </si>
+  <si>
+    <t>0.186</t>
+  </si>
+  <si>
+    <t>0.143</t>
+  </si>
+  <si>
+    <t>0.177</t>
+  </si>
+  <si>
+    <t>0.354</t>
+  </si>
+  <si>
+    <t>0.207</t>
+  </si>
+  <si>
+    <t>0.8</t>
+  </si>
+  <si>
+    <t>16.6</t>
+  </si>
+  <si>
+    <t>1.33</t>
   </si>
 </sst>
 </file>
@@ -221,7 +248,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -236,6 +263,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -551,10 +581,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDAA485E-46B0-0B4F-9545-40FBAD212A5C}">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -617,8 +647,8 @@
       <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="4">
-        <v>0.8</v>
+      <c r="D2" s="4" t="s">
+        <v>51</v>
       </c>
       <c r="E2" s="3">
         <v>26</v>
@@ -635,8 +665,8 @@
       <c r="I2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="3">
-        <v>0.186</v>
+      <c r="J2" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>43</v>
@@ -652,8 +682,8 @@
       <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="4">
-        <v>0.8</v>
+      <c r="D3" s="4" t="s">
+        <v>51</v>
       </c>
       <c r="E3" s="3">
         <v>26</v>
@@ -670,8 +700,8 @@
       <c r="I3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="3">
-        <v>0.14299999999999999</v>
+      <c r="J3" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="K3" s="3" t="s">
         <v>43</v>
@@ -687,8 +717,8 @@
       <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="4">
-        <v>1.33</v>
+      <c r="D4" s="6" t="s">
+        <v>53</v>
       </c>
       <c r="E4" s="3">
         <v>28</v>
@@ -705,8 +735,8 @@
       <c r="I4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J4" s="3">
-        <v>0.17699999999999999</v>
+      <c r="J4" s="3" t="s">
+        <v>48</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>43</v>
@@ -722,8 +752,8 @@
       <c r="C5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="4">
-        <v>0.8</v>
+      <c r="D5" s="4" t="s">
+        <v>51</v>
       </c>
       <c r="E5" s="3">
         <v>25</v>
@@ -740,8 +770,8 @@
       <c r="I5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="3">
-        <v>0.14299999999999999</v>
+      <c r="J5" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="K5" s="3" t="s">
         <v>43</v>
@@ -757,8 +787,8 @@
       <c r="C6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="4">
-        <v>0.8</v>
+      <c r="D6" s="4" t="s">
+        <v>51</v>
       </c>
       <c r="E6" s="3">
         <v>27</v>
@@ -775,8 +805,8 @@
       <c r="I6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J6" s="3">
-        <v>0.14299999999999999</v>
+      <c r="J6" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="K6" s="3" t="s">
         <v>43</v>
@@ -792,8 +822,8 @@
       <c r="C7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="4">
-        <v>0.8</v>
+      <c r="D7" s="4" t="s">
+        <v>51</v>
       </c>
       <c r="E7" s="3">
         <v>26</v>
@@ -810,8 +840,8 @@
       <c r="I7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J7" s="3">
-        <v>0.14299999999999999</v>
+      <c r="J7" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="K7" s="3" t="s">
         <v>43</v>
@@ -827,8 +857,8 @@
       <c r="C8" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="4">
-        <v>0.7</v>
+      <c r="D8" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="E8" s="3">
         <v>20</v>
@@ -845,8 +875,8 @@
       <c r="I8" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J8" s="3">
-        <v>0.35399999999999998</v>
+      <c r="J8" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="K8" s="3" t="s">
         <v>42</v>
@@ -880,8 +910,8 @@
       <c r="I9" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J9" s="3">
-        <v>0.20699999999999999</v>
+      <c r="J9" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="K9" s="5" t="s">
         <v>44</v>
@@ -915,8 +945,8 @@
       <c r="I10" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J10" s="3">
-        <v>0.20699999999999999</v>
+      <c r="J10" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="K10" s="5" t="s">
         <v>44</v>
@@ -950,8 +980,8 @@
       <c r="I11" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J11" s="3">
-        <v>0.20699999999999999</v>
+      <c r="J11" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="K11" s="5" t="s">
         <v>44</v>
@@ -967,11 +997,11 @@
       <c r="C12" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="E12" s="3">
-        <v>16.600000000000001</v>
+      <c r="D12" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>52</v>
       </c>
       <c r="F12" s="3">
         <v>19</v>
@@ -985,12 +1015,15 @@
       <c r="I12" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J12" s="3">
-        <v>0.20699999999999999</v>
+      <c r="J12" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="K12" s="5" t="s">
         <v>41</v>
       </c>
+    </row>
+    <row r="25" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C25" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>